<commit_message>
fix: actualizar mapeo columnas Excel compresion al nuevo template (eliminar Hora antigua, Hora Ensayo después de Fecha revisado)
</commit_message>
<xml_diff>
--- a/app/templates/Template_Compresion.xlsx
+++ b/app/templates/Template_Compresion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DECAA16-78EE-4D45-8EE7-3255DF821FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBD0218-2957-4A2A-B697-670DC3C2C19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,6 +641,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -653,45 +692,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1158,8 +1158,8 @@
       <xdr:rowOff>75275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>47446</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>580846</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>141950</xdr:rowOff>
     </xdr:to>
@@ -1567,8 +1567,8 @@
   </sheetPr>
   <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1578,7 +1578,7 @@
     <col min="3" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" style="1" customWidth="1"/>
     <col min="10" max="13" width="9.109375" style="1" customWidth="1"/>
@@ -1687,44 +1687,44 @@
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
     </row>
     <row r="8" spans="1:26" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="V8" s="60"/>
-      <c r="W8" s="60"/>
-      <c r="X8" s="60"/>
-      <c r="Y8" s="60"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="V8" s="70"/>
+      <c r="W8" s="70"/>
+      <c r="X8" s="70"/>
+      <c r="Y8" s="70"/>
       <c r="Z8" s="15"/>
     </row>
     <row r="9" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1740,10 +1740,10 @@
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
-      <c r="V9" s="60"/>
-      <c r="W9" s="60"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="60"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
+      <c r="Y9" s="70"/>
       <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1767,47 +1767,47 @@
       <c r="N11" s="13"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="S11" s="64"/>
-      <c r="T11" s="64"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="60"/>
     </row>
     <row r="12" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="67"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="63"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="69"/>
-      <c r="N13" s="70"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="66"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -1827,25 +1827,25 @@
         <v>20</v>
       </c>
       <c r="E15" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="43" t="s">
         <v>7</v>
-      </c>
-      <c r="F15" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="43" t="s">
-        <v>18</v>
       </c>
       <c r="L15" s="43" t="s">
         <v>16</v>
@@ -2195,8 +2195,8 @@
       <c r="T33" s="20"/>
       <c r="U33" s="20"/>
       <c r="V33" s="20"/>
-      <c r="W33" s="59"/>
-      <c r="X33" s="59"/>
+      <c r="W33" s="69"/>
+      <c r="X33" s="69"/>
     </row>
     <row r="34" spans="1:27" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="35"/>
@@ -2224,18 +2224,18 @@
     <row r="35" spans="1:27" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="35"/>
       <c r="B35" s="35"/>
-      <c r="C35" s="61" t="s">
+      <c r="C35" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="61"/>
+      <c r="D35" s="57"/>
       <c r="E35" s="56"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
       <c r="H35" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
+      <c r="I35" s="58"/>
+      <c r="J35" s="58"/>
       <c r="P35" s="3"/>
       <c r="Q35" s="19"/>
       <c r="R35" s="28"/>
@@ -2346,27 +2346,34 @@
     </row>
     <row r="41" spans="1:27" ht="13.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:27" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="63" t="s">
+      <c r="A42" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="63"/>
-      <c r="I42" s="63"/>
-      <c r="J42" s="63"/>
-      <c r="K42" s="63"/>
-      <c r="L42" s="63"/>
-      <c r="M42" s="63"/>
-      <c r="N42" s="63"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
     </row>
     <row r="43" spans="1:27" ht="15.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:27" ht="15.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A7:N7"/>
+    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:Y9"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="I35:J35"/>
@@ -2374,13 +2381,6 @@
     <mergeCell ref="S11:T11"/>
     <mergeCell ref="A12:N12"/>
     <mergeCell ref="A13:N13"/>
-    <mergeCell ref="A7:N7"/>
-    <mergeCell ref="A8:N8"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:Y9"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.39370078740157483" header="0" footer="0"/>

</xml_diff>

<commit_message>
feat: nuevo formato nombre Excel recepción: REC N-XXX-26 (NOMBRE EMPRESA)
</commit_message>
<xml_diff>
--- a/app/templates/Template_Compresion.xlsx
+++ b/app/templates/Template_Compresion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBD0218-2957-4A2A-B697-670DC3C2C19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC946D67-3543-4B91-A60C-9859211B861B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1567,8 +1567,8 @@
   </sheetPr>
   <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1839,13 +1839,13 @@
         <v>21</v>
       </c>
       <c r="I15" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="43" t="s">
         <v>17</v>
-      </c>
-      <c r="J15" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="43" t="s">
-        <v>7</v>
       </c>
       <c r="L15" s="43" t="s">
         <v>16</v>

</xml_diff>